<commit_message>
update status code + fix mapping b5e29ac10a83ce72a0a8133c72c08c8400972cc9
</commit_message>
<xml_diff>
--- a/389-mapping---projet-personnalisé/ig/StructureDefinition-tddui-careplan-projet-personnalise.xlsx
+++ b/389-mapping---projet-personnalisé/ig/StructureDefinition-tddui-careplan-projet-personnalise.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-03T10:22:03+00:00</t>
+    <t>2025-12-05T09:54:12+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -956,7 +956,7 @@
     <t>CarePlan.status</t>
   </si>
   <si>
-    <t>draft | active | on-hold | revoked | completed | entered-in-error | unknown</t>
+    <t>Correspondance des statuts métier avec les codes FHIR : ENPREPARATION → draft, ENCOURS → active, ENPAUSE → on-hold, TERMINE → completed.</t>
   </si>
   <si>
     <t>Indicates whether the plan is currently being acted upon, represents future intentions or is now a historical record.</t>

</xml_diff>